<commit_message>
update with new downscaled data
</commit_message>
<xml_diff>
--- a/Downscaleddata/pdfs/bottom o2_thresholds.xlsx
+++ b/Downscaleddata/pdfs/bottom o2_thresholds.xlsx
@@ -490,34 +490,34 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>3.371985294125172</v>
+        <v>3.371985244661392</v>
       </c>
       <c r="C2" t="n">
-        <v>1.100385064871179</v>
+        <v>1.100385049623747</v>
       </c>
       <c r="D2" t="n">
-        <v>3.195530200612898</v>
+        <v>3.542583507443938</v>
       </c>
       <c r="E2" t="n">
-        <v>1.196910142261056</v>
+        <v>1.034636339911349</v>
       </c>
       <c r="F2" t="n">
-        <v>3.171945884630063</v>
+        <v>3.524883908303043</v>
       </c>
       <c r="G2" t="n">
-        <v>1.166983854326101</v>
+        <v>0.628470476361786</v>
       </c>
       <c r="H2" t="n">
-        <v>3.172380132000818</v>
+        <v>3.347340434915449</v>
       </c>
       <c r="I2" t="n">
-        <v>1.236971766849623</v>
+        <v>0.9062051373079006</v>
       </c>
       <c r="J2" t="n">
-        <v>3.165496956178273</v>
+        <v>3.323262318674384</v>
       </c>
       <c r="K2" t="n">
-        <v>1.127675843754151</v>
+        <v>0.6290185522913129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced negative values for bottom O2
</commit_message>
<xml_diff>
--- a/Downscaleddata/pdfs/bottom o2_thresholds.xlsx
+++ b/Downscaleddata/pdfs/bottom o2_thresholds.xlsx
@@ -499,25 +499,25 @@
         <v>3.542583507443938</v>
       </c>
       <c r="E2" t="n">
-        <v>1.034636339911349</v>
+        <v>1.045389290513603</v>
       </c>
       <c r="F2" t="n">
         <v>3.524883908303043</v>
       </c>
       <c r="G2" t="n">
-        <v>0.628470476361786</v>
+        <v>0.6629871557899286</v>
       </c>
       <c r="H2" t="n">
         <v>3.347340434915449</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9062051373079006</v>
+        <v>0.9275548951266984</v>
       </c>
       <c r="J2" t="n">
-        <v>3.323262318674384</v>
+        <v>3.323323020455365</v>
       </c>
       <c r="K2" t="n">
-        <v>0.6290185522913129</v>
+        <v>0.6758592141011408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>